<commit_message>
New updates on app properties
</commit_message>
<xml_diff>
--- a/forms/contact/household_member-create.xlsx
+++ b/forms/contact/household_member-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="175">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">contact_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_contact</t>
   </si>
   <si>
     <t xml:space="preserve">Names</t>
@@ -955,8 +958,8 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.29296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1435,7 +1438,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="5"/>
       <c r="N12" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -1459,13 +1462,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -1474,16 +1477,16 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>17</v>
@@ -1495,7 +1498,7 @@
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
@@ -1509,10 +1512,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1528,23 +1531,23 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1555,16 +1558,16 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1572,7 +1575,7 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -1580,23 +1583,23 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -1607,25 +1610,25 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1636,29 +1639,29 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -1667,43 +1670,43 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>17</v>
@@ -1725,10 +1728,10 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>17</v>
@@ -1740,7 +1743,7 @@
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
@@ -1748,10 +1751,10 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>17</v>
@@ -1763,7 +1766,7 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
@@ -1771,10 +1774,10 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>17</v>
@@ -1786,7 +1789,7 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
@@ -1794,10 +1797,10 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>17</v>
@@ -1809,7 +1812,7 @@
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -1817,10 +1820,10 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>17</v>
@@ -1832,7 +1835,7 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
@@ -1840,10 +1843,10 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>17</v>
@@ -1855,7 +1858,7 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -1863,10 +1866,10 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>17</v>
@@ -1878,7 +1881,7 @@
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
@@ -1886,16 +1889,16 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="11" t="b">
@@ -1912,20 +1915,20 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="12" t="n">
@@ -1933,31 +1936,31 @@
         <v>1</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="12" t="n">
@@ -1965,30 +1968,30 @@
         <v>1</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -2001,22 +2004,22 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -2031,7 +2034,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>17</v>
@@ -2070,7 +2073,7 @@
         <v>28</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>17</v>
@@ -2089,7 +2092,7 @@
       <c r="M36" s="5"/>
       <c r="N36" s="4"/>
       <c r="O36" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
@@ -2109,7 +2112,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>17</v>
@@ -2146,7 +2149,7 @@
         <v>28</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>17</v>
@@ -2180,10 +2183,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="5"/>
@@ -2193,14 +2196,14 @@
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="5"/>
       <c r="N39" s="4"/>
       <c r="O39" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
@@ -2217,10 +2220,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
@@ -2230,7 +2233,7 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
@@ -2252,10 +2255,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="5"/>
@@ -2265,7 +2268,7 @@
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -30142,7 +30145,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
@@ -30155,7 +30158,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
@@ -30188,16 +30191,16 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -30221,16 +30224,16 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -30254,16 +30257,16 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -30287,16 +30290,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -30320,16 +30323,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -30353,16 +30356,16 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -30386,16 +30389,16 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -30419,16 +30422,16 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -30452,16 +30455,16 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -30485,16 +30488,16 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -30518,16 +30521,16 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -30551,16 +30554,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -30584,30 +30587,30 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -31606,8 +31609,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.29296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31624,19 +31627,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="3"/>
@@ -31662,20 +31665,20 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C2" s="25" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-07-31  14-43</v>
+        <v>2023-11-29  10-14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>

</xml_diff>